<commit_message>
Craete new Register class
</commit_message>
<xml_diff>
--- a/Test Data/UserDetail.xlsx
+++ b/Test Data/UserDetail.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinot\eclipse-workspace\IXPerformers\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBB7755-1C91-488D-BD00-978B7079C3DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4056BD6A-FD58-46BF-BEA8-70249D0C1804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6EA6832E-1083-47CC-A076-D466552BB0F2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{6EA6832E-1083-47CC-A076-D466552BB0F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Coach" sheetId="1" r:id="rId1"/>
-    <sheet name="Player" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="Player" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="99">
   <si>
     <t>First Name</t>
   </si>
@@ -236,13 +238,109 @@
   </si>
   <si>
     <t>T@gmail.com</t>
+  </si>
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>Email Address</t>
+  </si>
+  <si>
+    <t>Academy Name</t>
+  </si>
+  <si>
+    <t>FIrst Name</t>
+  </si>
+  <si>
+    <t>Email ID (For Login)</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>Specialized in</t>
+  </si>
+  <si>
+    <t>Educational Qualification</t>
+  </si>
+  <si>
+    <t>Experience</t>
+  </si>
+  <si>
+    <t>Sp [Row 1]</t>
+  </si>
+  <si>
+    <t>11/27/2025 18:52:16</t>
+  </si>
+  <si>
+    <t>XIFT Academy and Research</t>
+  </si>
+  <si>
+    <t>11/27/2000</t>
+  </si>
+  <si>
+    <t>College Roll/ID Number</t>
+  </si>
+  <si>
+    <t>Parental Relatonship</t>
+  </si>
+  <si>
+    <t>Parent / Guardian Name</t>
+  </si>
+  <si>
+    <t>Parent Mobile Number</t>
+  </si>
+  <si>
+    <t>Sub Events</t>
+  </si>
+  <si>
+    <t>Name of the School or College</t>
+  </si>
+  <si>
+    <t>Board (If School)</t>
+  </si>
+  <si>
+    <t>Degree (If College)</t>
+  </si>
+  <si>
+    <t>Standard (If School)</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>oth</t>
+  </si>
+  <si>
+    <t>Arun Appavo</t>
+  </si>
+  <si>
+    <t>60 m, 4x100 m Relay, High Jump, Cricket</t>
+  </si>
+  <si>
+    <t>Discus Throw,  200 m, Cricket</t>
+  </si>
+  <si>
+    <t>santhosh@gmail.com</t>
+  </si>
+  <si>
+    <t>santhosh</t>
+  </si>
+  <si>
+    <t>dhoni@gmail.com</t>
+  </si>
+  <si>
+    <t>dhoni</t>
+  </si>
+  <si>
+    <t>ms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,8 +382,40 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Google Sans Mono"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF252C32"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -298,11 +428,43 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4285F4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -312,7 +474,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -340,6 +502,29 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -657,11 +842,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E6B11DD-29B1-4D40-8E89-CDB7BF8D325C}">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="22.109375" customWidth="1"/>
     <col min="2" max="2" width="24.5546875" customWidth="1"/>
@@ -682,7 +867,7 @@
     <col min="18" max="18" width="28.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="15.6">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -738,7 +923,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -794,7 +979,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -850,7 +1035,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -906,7 +1091,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -962,10 +1147,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18">
       <c r="C7" s="4"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18">
       <c r="B13" s="5"/>
     </row>
   </sheetData>
@@ -980,14 +1165,263 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F6E2CD-2474-4007-B3E8-FDB4020CC9CB}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" customWidth="1"/>
+    <col min="7" max="7" width="36" customWidth="1"/>
+    <col min="8" max="8" width="24.44140625" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" customWidth="1"/>
+    <col min="10" max="10" width="25.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="54" thickBot="1">
+      <c r="A1" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" s="14"/>
+    </row>
+    <row r="2" spans="1:14" ht="54" thickBot="1">
+      <c r="A2" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="15">
+        <v>1234567895</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="15">
+        <v>56</v>
+      </c>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{9C4B22D1-37C8-41B1-AD06-F2632812BD32}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{2CBD781B-1134-46A7-AC9F-F02BAD5A4ADA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727DBF69-8735-4ABE-8D39-A3F9DD88817B}">
+  <dimension ref="A1:V2"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="16.77734375" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="22.33203125" customWidth="1"/>
+    <col min="13" max="13" width="34.44140625" customWidth="1"/>
+    <col min="21" max="21" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="67.2" thickBot="1">
+      <c r="A1" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="S1" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="T1" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="U1" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="V1" s="19"/>
+    </row>
+    <row r="2" spans="1:22" ht="30">
+      <c r="C2" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2">
+        <v>12345</v>
+      </c>
+      <c r="G2">
+        <v>1234567890</v>
+      </c>
+      <c r="H2" s="1">
+        <v>35345</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="8">
+        <v>8675798564</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="U2" r:id="rId1" xr:uid="{9657B55C-1748-460A-9257-B305AFA5644F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C560751-74F1-4256-A600-3B451BA971D6}">
   <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9.88671875" customWidth="1"/>
     <col min="2" max="2" width="15.88671875" customWidth="1"/>
@@ -1013,7 +1447,7 @@
     <col min="24" max="24" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="31.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1087,7 +1521,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24">
       <c r="A2" s="8" t="s">
         <v>35</v>
       </c>
@@ -1161,7 +1595,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24">
       <c r="A3" s="8" t="s">
         <v>35</v>
       </c>
@@ -1231,7 +1665,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24">
       <c r="A4" s="8" t="s">
         <v>54</v>
       </c>
@@ -1303,7 +1737,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:5">
       <c r="E21" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
get the user id and annd updating the methods
</commit_message>
<xml_diff>
--- a/Test Data/UserDetail.xlsx
+++ b/Test Data/UserDetail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinot\eclipse-workspace\IXPerformers\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4056BD6A-FD58-46BF-BEA8-70249D0C1804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399169E8-7334-4C62-BECC-F7A589E2A71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{6EA6832E-1083-47CC-A076-D466552BB0F2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{6EA6832E-1083-47CC-A076-D466552BB0F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Coach" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="100">
   <si>
     <t>First Name</t>
   </si>
@@ -315,25 +315,28 @@
     <t>Arun Appavo</t>
   </si>
   <si>
-    <t>60 m, 4x100 m Relay, High Jump, Cricket</t>
-  </si>
-  <si>
-    <t>Discus Throw,  200 m, Cricket</t>
-  </si>
-  <si>
-    <t>santhosh@gmail.com</t>
-  </si>
-  <si>
     <t>santhosh</t>
   </si>
   <si>
-    <t>dhoni@gmail.com</t>
-  </si>
-  <si>
     <t>dhoni</t>
   </si>
   <si>
     <t>ms</t>
+  </si>
+  <si>
+    <t>60 m, 4x100 m Relay</t>
+  </si>
+  <si>
+    <t>TestXI5@gmail.com</t>
+  </si>
+  <si>
+    <t>Discus Throw,  200 m</t>
+  </si>
+  <si>
+    <t>TestXI25@gmail.com</t>
+  </si>
+  <si>
+    <t>TestXI26@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1168,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F6E2CD-2474-4007-B3E8-FDB4020CC9CB}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1236,13 +1239,13 @@
         <v>78</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E2" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="16" t="s">
         <v>98</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>96</v>
       </c>
       <c r="G2" s="15">
         <v>1234567895</v>
@@ -1254,7 +1257,7 @@
         <v>5</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="K2" t="s">
         <v>25</v>
@@ -1268,7 +1271,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{9C4B22D1-37C8-41B1-AD06-F2632812BD32}"/>
-    <hyperlink ref="F2" r:id="rId2" xr:uid="{2CBD781B-1134-46A7-AC9F-F02BAD5A4ADA}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{287232D7-D6AE-4D4A-B4A6-A0C4D3EF8A04}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1278,8 +1281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727DBF69-8735-4ABE-8D39-A3F9DD88817B}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1361,12 +1364,12 @@
       </c>
       <c r="V1" s="19"/>
     </row>
-    <row r="2" spans="1:22" ht="30">
+    <row r="2" spans="1:22" ht="30.6" thickBot="1">
       <c r="C2" s="21" t="s">
         <v>91</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
         <v>90</v>
@@ -1393,7 +1396,7 @@
         <v>8675798564</v>
       </c>
       <c r="M2" s="20" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="N2" s="8" t="s">
         <v>46</v>
@@ -1401,13 +1404,13 @@
       <c r="Q2" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="U2" s="2" t="s">
-        <v>94</v>
+      <c r="U2" s="16" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1" xr:uid="{9657B55C-1748-460A-9257-B305AFA5644F}"/>
+    <hyperlink ref="U2" r:id="rId1" xr:uid="{9769261A-0F01-48E0-9623-E65C20AE12E2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>